<commit_message>
Wallets completed postive scenarios
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -3,21 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intuitiveapps\eclipse-workspace\Kyce\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070395D5-F869-48E0-AF86-A9269ECE6308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2FF97034-47C8-43B8-AD87-931B5F260ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0AF623DB-6EC0-4448-B883-F3B446A1A0B1}"/>
+    <workbookView xWindow="1740" yWindow="5100" windowWidth="15660" windowHeight="8880" xr2:uid="{0AF623DB-6EC0-4448-B883-F3B446A1A0B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -548,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0780A1FF-5AFA-40D2-A2B0-E6778936ABA9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -660,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B792F02-2433-4C15-813F-15C48A5D0F13}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>